<commit_message>
Remove some sequences from O random samples, Add trees for serotype A without outliers
</commit_message>
<xml_diff>
--- a/Tables/Best_model_table.xlsx
+++ b/Tables/Best_model_table.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>Serotype</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>SAT3</t>
-  </si>
-  <si>
-    <t>Coalescent Exponential Population, Strict clock</t>
   </si>
   <si>
     <t>Coalescent Bayesian Skyline, Relaxed clock Lognormal</t>
@@ -394,7 +391,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +420,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -431,7 +428,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -439,7 +436,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -447,7 +444,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -455,7 +452,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -463,7 +460,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>